<commit_message>
updated data element templates
</commit_message>
<xml_diff>
--- a/cdes/RADx-rad_Min_CDE _Data_Element_Template_v003.xlsx
+++ b/cdes/RADx-rad_Min_CDE _Data_Element_Template_v003.xlsx
@@ -696,9 +696,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="3" width="14.89"/>
-    <col customWidth="1" min="4" max="4" width="17.56"/>
-    <col customWidth="1" min="5" max="12" width="14.89"/>
+    <col customWidth="1" min="1" max="1" width="23.0"/>
+    <col customWidth="1" min="2" max="3" width="14.89"/>
+    <col customWidth="1" min="4" max="4" width="22.11"/>
+    <col customWidth="1" min="5" max="5" width="33.56"/>
+    <col customWidth="1" min="6" max="6" width="14.89"/>
+    <col customWidth="1" min="7" max="7" width="11.89"/>
+    <col customWidth="1" min="8" max="12" width="14.89"/>
     <col customWidth="1" min="13" max="26" width="10.56"/>
   </cols>
   <sheetData>

</xml_diff>